<commit_message>
Edit payment in 20231117
</commit_message>
<xml_diff>
--- a/data/checked/player/20231117_listplayer.xlsx
+++ b/data/checked/player/20231117_listplayer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\badminton-payment\player\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1dd2fc4bf918acb/Projects/badminton-payment2/player/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78515E5-5471-4DAE-8B17-C47630C2067A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{D78515E5-5471-4DAE-8B17-C47630C2067A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B11BE16-7336-438E-A9CF-FCAAD163AD28}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023xxxx_listplayer" sheetId="1" r:id="rId1"/>
@@ -1315,7 +1315,7 @@
         <v>57</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1359,7 +1359,7 @@
         <v>57</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1381,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="L7" t="s">
         <v>96</v>
@@ -1406,7 +1406,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1494,7 +1494,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2044,7 +2044,7 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2484,7 +2484,7 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2638,7 +2638,7 @@
         <v>0</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2671,7 +2671,7 @@
         <v>84</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" ref="C66:C97" si="2">_xlfn.CONCAT(B66,A66)</f>
+        <f t="shared" ref="C66:C67" si="2">_xlfn.CONCAT(B66,A66)</f>
         <v>NuengSCM</v>
       </c>
       <c r="D66">
@@ -2704,7 +2704,7 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>